<commit_message>
README virtual_env edits/template tweaks
</commit_message>
<xml_diff>
--- a/proc-card-log-TEMPLATE.xlsx
+++ b/proc-card-log-TEMPLATE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trb74/Box Sync/ERS Shared/Innovative - Sierra/EDIFACT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trb74/github/xls2inv/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -431,11 +431,6 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
-      <formula1>"PC-DAWN,PC-ZENY,PC-OLYU"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>